<commit_message>
Redo TODC school-age norms with new sample
</commit_message>
<xml_diff>
--- a/OUTPUT-FILES/NORMS/TODC_final_gr1_12_10.28.21_fornorms/seg_sum-raw-ss-lookup-tabbed-age.xlsx
+++ b/OUTPUT-FILES/NORMS/TODC_final_gr1_12_10.28.21_fornorms/seg_sum-raw-ss-lookup-tabbed-age.xlsx
@@ -401,7 +401,7 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="4">
@@ -441,7 +441,7 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="9">
@@ -449,7 +449,7 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="10">
@@ -457,7 +457,7 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="11">
@@ -473,7 +473,7 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="13">
@@ -481,7 +481,7 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="14">
@@ -489,7 +489,7 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="15">
@@ -497,7 +497,7 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="16">
@@ -505,7 +505,7 @@
         <v>14</v>
       </c>
       <c r="B16">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="17">
@@ -513,7 +513,7 @@
         <v>15</v>
       </c>
       <c r="B17">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="18">
@@ -521,7 +521,7 @@
         <v>16</v>
       </c>
       <c r="B18">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="19">
@@ -529,7 +529,7 @@
         <v>17</v>
       </c>
       <c r="B19">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="20">
@@ -537,7 +537,7 @@
         <v>18</v>
       </c>
       <c r="B20">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="21">
@@ -545,7 +545,7 @@
         <v>19</v>
       </c>
       <c r="B21">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="22">
@@ -553,7 +553,7 @@
         <v>20</v>
       </c>
       <c r="B22">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="23">
@@ -561,7 +561,7 @@
         <v>21</v>
       </c>
       <c r="B23">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="24">
@@ -569,7 +569,7 @@
         <v>22</v>
       </c>
       <c r="B24">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="25">
@@ -577,7 +577,7 @@
         <v>23</v>
       </c>
       <c r="B25">
-        <v>124</v>
+        <v>121</v>
       </c>
     </row>
     <row r="26">
@@ -585,7 +585,7 @@
         <v>24</v>
       </c>
       <c r="B26">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="27">
@@ -593,7 +593,7 @@
         <v>25</v>
       </c>
       <c r="B27">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="28">
@@ -658,7 +658,7 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3">
@@ -666,7 +666,7 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
     <row r="4">
@@ -674,7 +674,7 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5">
@@ -682,7 +682,7 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
     <row r="6">
@@ -690,7 +690,7 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="7">
@@ -698,7 +698,7 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="8">
@@ -706,7 +706,7 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="9">
@@ -714,7 +714,7 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="10">
@@ -722,7 +722,7 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="11">
@@ -730,7 +730,7 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="12">
@@ -738,7 +738,7 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="13">
@@ -746,7 +746,7 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="14">
@@ -754,7 +754,7 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="15">
@@ -762,7 +762,7 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="16">
@@ -770,7 +770,7 @@
         <v>14</v>
       </c>
       <c r="B16">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="17">
@@ -778,7 +778,7 @@
         <v>15</v>
       </c>
       <c r="B17">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="18">
@@ -786,7 +786,7 @@
         <v>16</v>
       </c>
       <c r="B18">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="19">
@@ -802,7 +802,7 @@
         <v>18</v>
       </c>
       <c r="B20">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="21">
@@ -850,7 +850,7 @@
         <v>24</v>
       </c>
       <c r="B26">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="27">
@@ -858,7 +858,7 @@
         <v>25</v>
       </c>
       <c r="B27">
-        <v>120</v>
+        <v>121</v>
       </c>
     </row>
     <row r="28">
@@ -866,7 +866,7 @@
         <v>26</v>
       </c>
       <c r="B28">
-        <v>124</v>
+        <v>125</v>
       </c>
     </row>
     <row r="29">
@@ -874,7 +874,7 @@
         <v>27</v>
       </c>
       <c r="B29">
-        <v>128</v>
+        <v>129</v>
       </c>
     </row>
     <row r="30">
@@ -923,7 +923,7 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3">
@@ -931,7 +931,7 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>45</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4">
@@ -939,7 +939,7 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="5">
@@ -947,7 +947,7 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="6">
@@ -955,7 +955,7 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
     <row r="7">
@@ -963,7 +963,7 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>55</v>
+        <v>51</v>
       </c>
     </row>
     <row r="8">
@@ -971,7 +971,7 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="9">
@@ -979,7 +979,7 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="10">
@@ -987,7 +987,7 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="11">
@@ -995,7 +995,7 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="12">
@@ -1003,7 +1003,7 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="13">
@@ -1011,7 +1011,7 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="14">
@@ -1019,7 +1019,7 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="15">
@@ -1027,7 +1027,7 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="16">
@@ -1035,7 +1035,7 @@
         <v>14</v>
       </c>
       <c r="B16">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="17">
@@ -1043,7 +1043,7 @@
         <v>15</v>
       </c>
       <c r="B17">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="18">
@@ -1051,7 +1051,7 @@
         <v>16</v>
       </c>
       <c r="B18">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="19">
@@ -1067,7 +1067,7 @@
         <v>18</v>
       </c>
       <c r="B20">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="21">
@@ -1083,7 +1083,7 @@
         <v>20</v>
       </c>
       <c r="B22">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="23">
@@ -1123,7 +1123,7 @@
         <v>25</v>
       </c>
       <c r="B27">
-        <v>119</v>
+        <v>120</v>
       </c>
     </row>
     <row r="28">
@@ -1131,7 +1131,7 @@
         <v>26</v>
       </c>
       <c r="B28">
-        <v>123</v>
+        <v>124</v>
       </c>
     </row>
     <row r="29">
@@ -1139,7 +1139,7 @@
         <v>27</v>
       </c>
       <c r="B29">
-        <v>127</v>
+        <v>128</v>
       </c>
     </row>
     <row r="30">
@@ -1188,7 +1188,7 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3">
@@ -1196,7 +1196,7 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4">
@@ -1204,7 +1204,7 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>46</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5">
@@ -1212,7 +1212,7 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="6">
@@ -1220,7 +1220,7 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
     <row r="7">
@@ -1228,7 +1228,7 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="8">
@@ -1236,7 +1236,7 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="9">
@@ -1244,7 +1244,7 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="10">
@@ -1252,7 +1252,7 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="11">
@@ -1260,7 +1260,7 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="12">
@@ -1268,7 +1268,7 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="13">
@@ -1276,7 +1276,7 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="14">
@@ -1284,7 +1284,7 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="15">
@@ -1292,7 +1292,7 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="16">
@@ -1300,7 +1300,7 @@
         <v>14</v>
       </c>
       <c r="B16">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="17">
@@ -1308,7 +1308,7 @@
         <v>15</v>
       </c>
       <c r="B17">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="18">
@@ -1316,7 +1316,7 @@
         <v>16</v>
       </c>
       <c r="B18">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="19">
@@ -1324,7 +1324,7 @@
         <v>17</v>
       </c>
       <c r="B19">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="20">
@@ -1332,7 +1332,7 @@
         <v>18</v>
       </c>
       <c r="B20">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="21">
@@ -1348,7 +1348,7 @@
         <v>20</v>
       </c>
       <c r="B22">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="23">
@@ -1461,7 +1461,7 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4">
@@ -1469,7 +1469,7 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>45</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5">
@@ -1477,7 +1477,7 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="6">
@@ -1485,7 +1485,7 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>50</v>
+        <v>46</v>
       </c>
     </row>
     <row r="7">
@@ -1493,7 +1493,7 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="8">
@@ -1501,7 +1501,7 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>55</v>
+        <v>51</v>
       </c>
     </row>
     <row r="9">
@@ -1509,7 +1509,7 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="10">
@@ -1517,7 +1517,7 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="11">
@@ -1525,7 +1525,7 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="12">
@@ -1533,7 +1533,7 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="13">
@@ -1541,7 +1541,7 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="14">
@@ -1549,7 +1549,7 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="15">
@@ -1557,7 +1557,7 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="16">
@@ -1565,7 +1565,7 @@
         <v>14</v>
       </c>
       <c r="B16">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="17">
@@ -1573,7 +1573,7 @@
         <v>15</v>
       </c>
       <c r="B17">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="18">
@@ -1581,7 +1581,7 @@
         <v>16</v>
       </c>
       <c r="B18">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="19">
@@ -1589,7 +1589,7 @@
         <v>17</v>
       </c>
       <c r="B19">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="20">
@@ -1597,7 +1597,7 @@
         <v>18</v>
       </c>
       <c r="B20">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="21">
@@ -1613,7 +1613,7 @@
         <v>20</v>
       </c>
       <c r="B22">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="23">
@@ -1621,7 +1621,7 @@
         <v>21</v>
       </c>
       <c r="B23">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="24">
@@ -1669,7 +1669,7 @@
         <v>27</v>
       </c>
       <c r="B29">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="30">
@@ -1726,7 +1726,7 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4">
@@ -1734,7 +1734,7 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5">
@@ -1742,7 +1742,7 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
     <row r="6">
@@ -1750,7 +1750,7 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>49</v>
+        <v>44</v>
       </c>
     </row>
     <row r="7">
@@ -1758,7 +1758,7 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
     <row r="8">
@@ -1766,7 +1766,7 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
     <row r="9">
@@ -1774,7 +1774,7 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="10">
@@ -1782,7 +1782,7 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="11">
@@ -1790,7 +1790,7 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="12">
@@ -1798,7 +1798,7 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="13">
@@ -1806,7 +1806,7 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="14">
@@ -1814,7 +1814,7 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="15">
@@ -1822,7 +1822,7 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="16">
@@ -1830,7 +1830,7 @@
         <v>14</v>
       </c>
       <c r="B16">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="17">
@@ -1838,7 +1838,7 @@
         <v>15</v>
       </c>
       <c r="B17">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="18">
@@ -1846,7 +1846,7 @@
         <v>16</v>
       </c>
       <c r="B18">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="19">
@@ -1854,7 +1854,7 @@
         <v>17</v>
       </c>
       <c r="B19">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="20">
@@ -1862,7 +1862,7 @@
         <v>18</v>
       </c>
       <c r="B20">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="21">
@@ -1886,7 +1886,7 @@
         <v>21</v>
       </c>
       <c r="B23">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="24">
@@ -1894,7 +1894,7 @@
         <v>22</v>
       </c>
       <c r="B24">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="25">
@@ -1902,7 +1902,7 @@
         <v>23</v>
       </c>
       <c r="B25">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="26">
@@ -1910,7 +1910,7 @@
         <v>24</v>
       </c>
       <c r="B26">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="27">
@@ -1918,7 +1918,7 @@
         <v>25</v>
       </c>
       <c r="B27">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="28">
@@ -1991,7 +1991,7 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4">
@@ -1999,7 +1999,7 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5">
@@ -2007,7 +2007,7 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>46</v>
+        <v>41</v>
       </c>
     </row>
     <row r="6">
@@ -2015,7 +2015,7 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>48</v>
+        <v>43</v>
       </c>
     </row>
     <row r="7">
@@ -2023,7 +2023,7 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>50</v>
+        <v>46</v>
       </c>
     </row>
     <row r="8">
@@ -2031,7 +2031,7 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>53</v>
+        <v>49</v>
       </c>
     </row>
     <row r="9">
@@ -2039,7 +2039,7 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>56</v>
+        <v>52</v>
       </c>
     </row>
     <row r="10">
@@ -2047,7 +2047,7 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="11">
@@ -2055,7 +2055,7 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="12">
@@ -2063,7 +2063,7 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="13">
@@ -2071,7 +2071,7 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="14">
@@ -2079,7 +2079,7 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="15">
@@ -2087,7 +2087,7 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="16">
@@ -2095,7 +2095,7 @@
         <v>14</v>
       </c>
       <c r="B16">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="17">
@@ -2103,7 +2103,7 @@
         <v>15</v>
       </c>
       <c r="B17">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="18">
@@ -2111,7 +2111,7 @@
         <v>16</v>
       </c>
       <c r="B18">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="19">
@@ -2127,7 +2127,7 @@
         <v>18</v>
       </c>
       <c r="B20">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="21">
@@ -2135,7 +2135,7 @@
         <v>19</v>
       </c>
       <c r="B21">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="22">
@@ -2264,7 +2264,7 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5">
@@ -2272,7 +2272,7 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>45</v>
+        <v>40</v>
       </c>
     </row>
     <row r="6">
@@ -2280,7 +2280,7 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="7">
@@ -2288,7 +2288,7 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>50</v>
+        <v>45</v>
       </c>
     </row>
     <row r="8">
@@ -2296,7 +2296,7 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
     <row r="9">
@@ -2304,7 +2304,7 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>55</v>
+        <v>51</v>
       </c>
     </row>
     <row r="10">
@@ -2312,7 +2312,7 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="11">
@@ -2320,7 +2320,7 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="12">
@@ -2328,7 +2328,7 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="13">
@@ -2336,7 +2336,7 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="14">
@@ -2344,7 +2344,7 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="15">
@@ -2352,7 +2352,7 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="16">
@@ -2360,7 +2360,7 @@
         <v>14</v>
       </c>
       <c r="B16">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="17">
@@ -2368,7 +2368,7 @@
         <v>15</v>
       </c>
       <c r="B17">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="18">
@@ -2376,7 +2376,7 @@
         <v>16</v>
       </c>
       <c r="B18">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="19">
@@ -2384,7 +2384,7 @@
         <v>17</v>
       </c>
       <c r="B19">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="20">
@@ -2400,7 +2400,7 @@
         <v>19</v>
       </c>
       <c r="B21">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="22">
@@ -2408,7 +2408,7 @@
         <v>20</v>
       </c>
       <c r="B22">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="23">
@@ -2416,7 +2416,7 @@
         <v>21</v>
       </c>
       <c r="B23">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="24">
@@ -2424,7 +2424,7 @@
         <v>22</v>
       </c>
       <c r="B24">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="25">
@@ -2432,7 +2432,7 @@
         <v>23</v>
       </c>
       <c r="B25">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="26">
@@ -2440,7 +2440,7 @@
         <v>24</v>
       </c>
       <c r="B26">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="27">
@@ -2448,7 +2448,7 @@
         <v>25</v>
       </c>
       <c r="B27">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="28">
@@ -2456,7 +2456,7 @@
         <v>26</v>
       </c>
       <c r="B28">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="29">
@@ -2464,7 +2464,7 @@
         <v>27</v>
       </c>
       <c r="B29">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="30">
@@ -2472,7 +2472,7 @@
         <v>28</v>
       </c>
       <c r="B30">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="31">
@@ -2529,7 +2529,7 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5">
@@ -2537,7 +2537,7 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="6">
@@ -2545,7 +2545,7 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>46</v>
+        <v>41</v>
       </c>
     </row>
     <row r="7">
@@ -2553,7 +2553,7 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="8">
@@ -2561,7 +2561,7 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
     <row r="9">
@@ -2569,7 +2569,7 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="10">
@@ -2577,7 +2577,7 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="11">
@@ -2585,7 +2585,7 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="12">
@@ -2593,7 +2593,7 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="13">
@@ -2601,7 +2601,7 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="14">
@@ -2609,7 +2609,7 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="15">
@@ -2617,7 +2617,7 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="16">
@@ -2625,7 +2625,7 @@
         <v>14</v>
       </c>
       <c r="B16">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="17">
@@ -2633,7 +2633,7 @@
         <v>15</v>
       </c>
       <c r="B17">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="18">
@@ -2641,7 +2641,7 @@
         <v>16</v>
       </c>
       <c r="B18">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="19">
@@ -2649,7 +2649,7 @@
         <v>17</v>
       </c>
       <c r="B19">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="20">
@@ -2665,7 +2665,7 @@
         <v>19</v>
       </c>
       <c r="B21">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="22">
@@ -2673,7 +2673,7 @@
         <v>20</v>
       </c>
       <c r="B22">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="23">
@@ -2681,7 +2681,7 @@
         <v>21</v>
       </c>
       <c r="B23">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="24">
@@ -2689,7 +2689,7 @@
         <v>22</v>
       </c>
       <c r="B24">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="25">
@@ -2697,7 +2697,7 @@
         <v>23</v>
       </c>
       <c r="B25">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="26">
@@ -2705,7 +2705,7 @@
         <v>24</v>
       </c>
       <c r="B26">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="27">
@@ -2713,7 +2713,7 @@
         <v>25</v>
       </c>
       <c r="B27">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="28">
@@ -2721,7 +2721,7 @@
         <v>26</v>
       </c>
       <c r="B28">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="29">
@@ -2729,7 +2729,7 @@
         <v>27</v>
       </c>
       <c r="B29">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="30">
@@ -2737,7 +2737,7 @@
         <v>28</v>
       </c>
       <c r="B30">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="31">
@@ -2802,7 +2802,7 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="6">
@@ -2810,7 +2810,7 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="7">
@@ -2818,7 +2818,7 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="8">
@@ -2826,7 +2826,7 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="9">
@@ -2834,7 +2834,7 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="10">
@@ -2842,7 +2842,7 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="11">
@@ -2850,7 +2850,7 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="12">
@@ -2858,7 +2858,7 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="13">
@@ -2866,7 +2866,7 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="14">
@@ -2882,7 +2882,7 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="16">
@@ -2938,7 +2938,7 @@
         <v>20</v>
       </c>
       <c r="B22">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="23">
@@ -2946,7 +2946,7 @@
         <v>21</v>
       </c>
       <c r="B23">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="24">
@@ -2954,7 +2954,7 @@
         <v>22</v>
       </c>
       <c r="B24">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="25">
@@ -2962,7 +2962,7 @@
         <v>23</v>
       </c>
       <c r="B25">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="26">
@@ -2970,7 +2970,7 @@
         <v>24</v>
       </c>
       <c r="B26">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="27">
@@ -2978,7 +2978,7 @@
         <v>25</v>
       </c>
       <c r="B27">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="28">
@@ -2986,7 +2986,7 @@
         <v>26</v>
       </c>
       <c r="B28">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="29">
@@ -2994,7 +2994,7 @@
         <v>27</v>
       </c>
       <c r="B29">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="30">
@@ -3002,7 +3002,7 @@
         <v>28</v>
       </c>
       <c r="B30">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="31">
@@ -3010,7 +3010,7 @@
         <v>29</v>
       </c>
       <c r="B31">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
   </sheetData>
@@ -3075,7 +3075,7 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="7">
@@ -3083,7 +3083,7 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="8">
@@ -3091,7 +3091,7 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="9">
@@ -3099,7 +3099,7 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="10">
@@ -3107,7 +3107,7 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="11">
@@ -3123,7 +3123,7 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="13">
@@ -3131,7 +3131,7 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="14">
@@ -3139,7 +3139,7 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="15">
@@ -3147,7 +3147,7 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="16">
@@ -3155,7 +3155,7 @@
         <v>14</v>
       </c>
       <c r="B16">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="17">
@@ -3163,7 +3163,7 @@
         <v>15</v>
       </c>
       <c r="B17">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="18">
@@ -3171,7 +3171,7 @@
         <v>16</v>
       </c>
       <c r="B18">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="19">
@@ -3179,7 +3179,7 @@
         <v>17</v>
       </c>
       <c r="B19">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="20">
@@ -3187,7 +3187,7 @@
         <v>18</v>
       </c>
       <c r="B20">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="21">
@@ -3219,7 +3219,7 @@
         <v>22</v>
       </c>
       <c r="B24">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="25">
@@ -3227,7 +3227,7 @@
         <v>23</v>
       </c>
       <c r="B25">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="26">
@@ -3235,7 +3235,7 @@
         <v>24</v>
       </c>
       <c r="B26">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="27">
@@ -3243,7 +3243,7 @@
         <v>25</v>
       </c>
       <c r="B27">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="28">
@@ -3251,7 +3251,7 @@
         <v>26</v>
       </c>
       <c r="B28">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="29">
@@ -3259,7 +3259,7 @@
         <v>27</v>
       </c>
       <c r="B29">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="30">
@@ -3267,7 +3267,7 @@
         <v>28</v>
       </c>
       <c r="B30">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="31">
@@ -3275,7 +3275,7 @@
         <v>29</v>
       </c>
       <c r="B31">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
   </sheetData>
@@ -3340,7 +3340,7 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="7">
@@ -3388,7 +3388,7 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="13">
@@ -3396,7 +3396,7 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="14">
@@ -3404,7 +3404,7 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="15">
@@ -3412,7 +3412,7 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="16">
@@ -3420,7 +3420,7 @@
         <v>14</v>
       </c>
       <c r="B16">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="17">
@@ -3428,7 +3428,7 @@
         <v>15</v>
       </c>
       <c r="B17">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="18">
@@ -3436,7 +3436,7 @@
         <v>16</v>
       </c>
       <c r="B18">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="19">
@@ -3444,7 +3444,7 @@
         <v>17</v>
       </c>
       <c r="B19">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="20">
@@ -3452,7 +3452,7 @@
         <v>18</v>
       </c>
       <c r="B20">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="21">
@@ -3460,7 +3460,7 @@
         <v>19</v>
       </c>
       <c r="B21">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="22">
@@ -3468,7 +3468,7 @@
         <v>20</v>
       </c>
       <c r="B22">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="23">
@@ -3476,7 +3476,7 @@
         <v>21</v>
       </c>
       <c r="B23">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="24">
@@ -3484,7 +3484,7 @@
         <v>22</v>
       </c>
       <c r="B24">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="25">
@@ -3492,7 +3492,7 @@
         <v>23</v>
       </c>
       <c r="B25">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="26">
@@ -3500,7 +3500,7 @@
         <v>24</v>
       </c>
       <c r="B26">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="27">
@@ -3508,7 +3508,7 @@
         <v>25</v>
       </c>
       <c r="B27">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="28">
@@ -3605,7 +3605,7 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="7">
@@ -3613,7 +3613,7 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
     <row r="8">
@@ -3621,7 +3621,7 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>45</v>
+        <v>48</v>
       </c>
     </row>
     <row r="9">
@@ -3629,7 +3629,7 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>47</v>
+        <v>51</v>
       </c>
     </row>
     <row r="10">
@@ -3637,7 +3637,7 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>50</v>
+        <v>54</v>
       </c>
     </row>
     <row r="11">
@@ -3645,7 +3645,7 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>53</v>
+        <v>57</v>
       </c>
     </row>
     <row r="12">
@@ -3653,7 +3653,7 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>56</v>
+        <v>60</v>
       </c>
     </row>
     <row r="13">
@@ -3661,7 +3661,7 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>59</v>
+        <v>64</v>
       </c>
     </row>
     <row r="14">
@@ -3669,7 +3669,7 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>62</v>
+        <v>67</v>
       </c>
     </row>
     <row r="15">
@@ -3677,7 +3677,7 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>66</v>
+        <v>71</v>
       </c>
     </row>
     <row r="16">
@@ -3685,7 +3685,7 @@
         <v>14</v>
       </c>
       <c r="B16">
-        <v>69</v>
+        <v>74</v>
       </c>
     </row>
     <row r="17">
@@ -3693,7 +3693,7 @@
         <v>15</v>
       </c>
       <c r="B17">
-        <v>73</v>
+        <v>77</v>
       </c>
     </row>
     <row r="18">
@@ -3701,7 +3701,7 @@
         <v>16</v>
       </c>
       <c r="B18">
-        <v>77</v>
+        <v>81</v>
       </c>
     </row>
     <row r="19">
@@ -3709,7 +3709,7 @@
         <v>17</v>
       </c>
       <c r="B19">
-        <v>81</v>
+        <v>84</v>
       </c>
     </row>
     <row r="20">
@@ -3717,7 +3717,7 @@
         <v>18</v>
       </c>
       <c r="B20">
-        <v>85</v>
+        <v>88</v>
       </c>
     </row>
     <row r="21">
@@ -3725,7 +3725,7 @@
         <v>19</v>
       </c>
       <c r="B21">
-        <v>89</v>
+        <v>91</v>
       </c>
     </row>
     <row r="22">
@@ -3733,7 +3733,7 @@
         <v>20</v>
       </c>
       <c r="B22">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="23">
@@ -3741,7 +3741,7 @@
         <v>21</v>
       </c>
       <c r="B23">
-        <v>96</v>
+        <v>98</v>
       </c>
     </row>
     <row r="24">
@@ -3749,7 +3749,7 @@
         <v>22</v>
       </c>
       <c r="B24">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row r="25">
@@ -3805,7 +3805,7 @@
         <v>29</v>
       </c>
       <c r="B31">
-        <v>122</v>
+        <v>123</v>
       </c>
     </row>
   </sheetData>
@@ -3838,7 +3838,7 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3">
@@ -3854,7 +3854,7 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="5">
@@ -3862,7 +3862,7 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="6">
@@ -3894,7 +3894,7 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="10">
@@ -3902,7 +3902,7 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="11">
@@ -3910,7 +3910,7 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="12">
@@ -3918,7 +3918,7 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="13">
@@ -3926,7 +3926,7 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="14">
@@ -3934,7 +3934,7 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="15">
@@ -3942,7 +3942,7 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="16">
@@ -3950,7 +3950,7 @@
         <v>14</v>
       </c>
       <c r="B16">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="17">
@@ -3958,7 +3958,7 @@
         <v>15</v>
       </c>
       <c r="B17">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="18">
@@ -3966,7 +3966,7 @@
         <v>16</v>
       </c>
       <c r="B18">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="19">
@@ -3974,7 +3974,7 @@
         <v>17</v>
       </c>
       <c r="B19">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="20">
@@ -3982,7 +3982,7 @@
         <v>18</v>
       </c>
       <c r="B20">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="21">
@@ -3990,7 +3990,7 @@
         <v>19</v>
       </c>
       <c r="B21">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="22">
@@ -3998,7 +3998,7 @@
         <v>20</v>
       </c>
       <c r="B22">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="23">
@@ -4006,7 +4006,7 @@
         <v>21</v>
       </c>
       <c r="B23">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="24">
@@ -4014,7 +4014,7 @@
         <v>22</v>
       </c>
       <c r="B24">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="25">
@@ -4022,7 +4022,7 @@
         <v>23</v>
       </c>
       <c r="B25">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="26">
@@ -4030,7 +4030,7 @@
         <v>24</v>
       </c>
       <c r="B26">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="27">
@@ -4038,7 +4038,7 @@
         <v>25</v>
       </c>
       <c r="B27">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="28">
@@ -4103,7 +4103,7 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="3">
@@ -4111,7 +4111,7 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="4">
@@ -4119,7 +4119,7 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="5">
@@ -4127,7 +4127,7 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="6">
@@ -4143,7 +4143,7 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="8">
@@ -4151,7 +4151,7 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="9">
@@ -4159,7 +4159,7 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="10">
@@ -4167,7 +4167,7 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="11">
@@ -4175,7 +4175,7 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="12">
@@ -4199,7 +4199,7 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="15">
@@ -4207,7 +4207,7 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="16">
@@ -4215,7 +4215,7 @@
         <v>14</v>
       </c>
       <c r="B16">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="17">
@@ -4223,7 +4223,7 @@
         <v>15</v>
       </c>
       <c r="B17">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="18">
@@ -4231,7 +4231,7 @@
         <v>16</v>
       </c>
       <c r="B18">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="19">
@@ -4239,7 +4239,7 @@
         <v>17</v>
       </c>
       <c r="B19">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="20">
@@ -4247,7 +4247,7 @@
         <v>18</v>
       </c>
       <c r="B20">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="21">
@@ -4255,7 +4255,7 @@
         <v>19</v>
       </c>
       <c r="B21">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="22">
@@ -4263,7 +4263,7 @@
         <v>20</v>
       </c>
       <c r="B22">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="23">
@@ -4271,7 +4271,7 @@
         <v>21</v>
       </c>
       <c r="B23">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="24">
@@ -4279,7 +4279,7 @@
         <v>22</v>
       </c>
       <c r="B24">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="25">
@@ -4287,7 +4287,7 @@
         <v>23</v>
       </c>
       <c r="B25">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="26">
@@ -4295,7 +4295,7 @@
         <v>24</v>
       </c>
       <c r="B26">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="27">
@@ -4303,7 +4303,7 @@
         <v>25</v>
       </c>
       <c r="B27">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="28">
@@ -4368,7 +4368,7 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3">
@@ -4376,7 +4376,7 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="4">
@@ -4384,7 +4384,7 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="5">
@@ -4392,7 +4392,7 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="6">
@@ -4400,7 +4400,7 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="7">
@@ -4408,7 +4408,7 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="8">
@@ -4416,7 +4416,7 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="9">
@@ -4424,7 +4424,7 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="10">
@@ -4440,7 +4440,7 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="12">
@@ -4448,7 +4448,7 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="13">
@@ -4456,7 +4456,7 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="14">
@@ -4488,7 +4488,7 @@
         <v>15</v>
       </c>
       <c r="B17">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="18">
@@ -4496,7 +4496,7 @@
         <v>16</v>
       </c>
       <c r="B18">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="19">
@@ -4504,7 +4504,7 @@
         <v>17</v>
       </c>
       <c r="B19">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="20">
@@ -4520,7 +4520,7 @@
         <v>19</v>
       </c>
       <c r="B21">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="22">
@@ -4528,7 +4528,7 @@
         <v>20</v>
       </c>
       <c r="B22">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="23">
@@ -4536,7 +4536,7 @@
         <v>21</v>
       </c>
       <c r="B23">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="24">
@@ -4544,7 +4544,7 @@
         <v>22</v>
       </c>
       <c r="B24">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="25">
@@ -4552,7 +4552,7 @@
         <v>23</v>
       </c>
       <c r="B25">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="26">
@@ -4568,7 +4568,7 @@
         <v>25</v>
       </c>
       <c r="B27">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="28">
@@ -4633,7 +4633,7 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3">
@@ -4641,7 +4641,7 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="4">
@@ -4649,7 +4649,7 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="5">
@@ -4657,7 +4657,7 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="6">
@@ -4665,7 +4665,7 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="7">
@@ -4673,7 +4673,7 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="8">
@@ -4681,7 +4681,7 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="9">
@@ -4689,7 +4689,7 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="10">
@@ -4697,7 +4697,7 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="11">
@@ -4705,7 +4705,7 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="12">
@@ -4713,7 +4713,7 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="13">
@@ -4721,7 +4721,7 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="14">
@@ -4729,7 +4729,7 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="15">
@@ -4737,7 +4737,7 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="16">
@@ -4761,7 +4761,7 @@
         <v>16</v>
       </c>
       <c r="B18">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="19">
@@ -4769,7 +4769,7 @@
         <v>17</v>
       </c>
       <c r="B19">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="20">
@@ -4785,7 +4785,7 @@
         <v>19</v>
       </c>
       <c r="B21">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="22">
@@ -4898,7 +4898,7 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3">
@@ -4906,7 +4906,7 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="4">
@@ -4914,7 +4914,7 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="5">
@@ -4922,7 +4922,7 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="6">
@@ -4930,7 +4930,7 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="7">
@@ -4938,7 +4938,7 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="8">
@@ -4946,7 +4946,7 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="9">
@@ -4954,7 +4954,7 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="10">
@@ -4962,7 +4962,7 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="11">
@@ -4970,7 +4970,7 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="12">
@@ -4978,7 +4978,7 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="13">
@@ -4986,7 +4986,7 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="14">
@@ -4994,7 +4994,7 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="15">
@@ -5002,7 +5002,7 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="16">
@@ -5010,7 +5010,7 @@
         <v>14</v>
       </c>
       <c r="B16">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="17">
@@ -5018,7 +5018,7 @@
         <v>15</v>
       </c>
       <c r="B17">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="18">
@@ -5034,7 +5034,7 @@
         <v>17</v>
       </c>
       <c r="B19">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="20">
@@ -5042,7 +5042,7 @@
         <v>18</v>
       </c>
       <c r="B20">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="21">
@@ -5058,7 +5058,7 @@
         <v>20</v>
       </c>
       <c r="B22">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="23">
@@ -5106,7 +5106,7 @@
         <v>26</v>
       </c>
       <c r="B28">
-        <v>127</v>
+        <v>128</v>
       </c>
     </row>
     <row r="29">
@@ -5163,7 +5163,7 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="3">
@@ -5171,7 +5171,7 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="4">
@@ -5179,7 +5179,7 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="5">
@@ -5187,7 +5187,7 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="6">
@@ -5195,7 +5195,7 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="7">
@@ -5203,7 +5203,7 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="8">
@@ -5211,7 +5211,7 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="9">
@@ -5219,7 +5219,7 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="10">
@@ -5227,7 +5227,7 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="11">
@@ -5235,7 +5235,7 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="12">
@@ -5243,7 +5243,7 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="13">
@@ -5251,7 +5251,7 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="14">
@@ -5259,7 +5259,7 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="15">
@@ -5267,7 +5267,7 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="16">
@@ -5283,7 +5283,7 @@
         <v>15</v>
       </c>
       <c r="B17">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="18">
@@ -5291,7 +5291,7 @@
         <v>16</v>
       </c>
       <c r="B18">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="19">
@@ -5315,7 +5315,7 @@
         <v>19</v>
       </c>
       <c r="B21">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="22">
@@ -5363,7 +5363,7 @@
         <v>25</v>
       </c>
       <c r="B27">
-        <v>122</v>
+        <v>123</v>
       </c>
     </row>
     <row r="28">
@@ -5371,7 +5371,7 @@
         <v>26</v>
       </c>
       <c r="B28">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="29">
@@ -5428,7 +5428,7 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3">
@@ -5436,7 +5436,7 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4">
@@ -5444,7 +5444,7 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="5">
@@ -5452,7 +5452,7 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="6">
@@ -5460,7 +5460,7 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="7">
@@ -5468,7 +5468,7 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="8">
@@ -5476,7 +5476,7 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="9">
@@ -5484,7 +5484,7 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="10">
@@ -5492,7 +5492,7 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="11">
@@ -5500,7 +5500,7 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="12">
@@ -5508,7 +5508,7 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="13">
@@ -5516,7 +5516,7 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="14">
@@ -5524,7 +5524,7 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="15">
@@ -5532,7 +5532,7 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="16">
@@ -5540,7 +5540,7 @@
         <v>14</v>
       </c>
       <c r="B16">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="17">
@@ -5548,7 +5548,7 @@
         <v>15</v>
       </c>
       <c r="B17">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="18">
@@ -5564,7 +5564,7 @@
         <v>17</v>
       </c>
       <c r="B19">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="20">
@@ -5620,7 +5620,7 @@
         <v>24</v>
       </c>
       <c r="B26">
-        <v>117</v>
+        <v>118</v>
       </c>
     </row>
     <row r="27">
@@ -5628,7 +5628,7 @@
         <v>25</v>
       </c>
       <c r="B27">
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
     <row r="28">
@@ -5636,7 +5636,7 @@
         <v>26</v>
       </c>
       <c r="B28">
-        <v>125</v>
+        <v>126</v>
       </c>
     </row>
     <row r="29">
@@ -5644,7 +5644,7 @@
         <v>27</v>
       </c>
       <c r="B29">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="30">

</xml_diff>